<commit_message>
Update Mock 2 with recent test data
</commit_message>
<xml_diff>
--- a/Results/Mock 2.xlsx
+++ b/Results/Mock 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\results giver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A430E635-498E-443C-9F5D-FE53C070E662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB76E60-6F27-4F35-8EC5-BF47112458A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -744,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -799,9 +799,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,7 +1137,7 @@
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+      <selection activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1258,32 +1255,32 @@
         <v>3</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <f t="shared" ref="M2:M19" si="4">K2*1 + L2*($Z$6)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N2">
         <f t="shared" ref="N2:N31" si="5">M2/$Y$3*100</f>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="O2">
         <f t="shared" ref="O2:O31" si="6">E2 + I2 + M2</f>
-        <v>8.75</v>
+        <v>13.75</v>
       </c>
       <c r="P2">
         <f t="shared" ref="P2:P31" si="7">O2/$Y$4*100</f>
-        <v>12.5</v>
+        <v>19.642857142857142</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q31" si="8">_xlfn.RANK.EQ(P2, $P$2:$P$1000, 0)</f>
-        <v>9</v>
-      </c>
-      <c r="R2" s="19">
+        <v>7</v>
+      </c>
+      <c r="R2" s="10">
         <v>21.5</v>
       </c>
       <c r="S2" s="11"/>
@@ -1291,7 +1288,7 @@
       <c r="U2" s="11"/>
       <c r="V2">
         <f t="shared" ref="V2:V11" si="9">O2+R2+S2+T2+U2</f>
-        <v>30.25</v>
+        <v>35.25</v>
       </c>
       <c r="W2">
         <f t="shared" ref="W2:W31" si="10">_xlfn.RANK.EQ(V2, $V$2:$V$1000, 0)</f>
@@ -1340,32 +1337,32 @@
         <v>-8</v>
       </c>
       <c r="K3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L3">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="M3">
         <f t="shared" si="4"/>
-        <v>1.25</v>
+        <v>6.25</v>
       </c>
       <c r="N3">
         <f t="shared" si="5"/>
-        <v>8.3333333333333321</v>
+        <v>41.666666666666671</v>
       </c>
       <c r="O3">
         <f t="shared" si="6"/>
-        <v>2.25</v>
+        <v>7.25</v>
       </c>
       <c r="P3">
         <f t="shared" si="7"/>
-        <v>3.214285714285714</v>
+        <v>10.357142857142858</v>
       </c>
       <c r="Q3">
         <f t="shared" si="8"/>
-        <v>13</v>
-      </c>
-      <c r="R3" s="19">
+        <v>12</v>
+      </c>
+      <c r="R3" s="10">
         <v>17</v>
       </c>
       <c r="S3" s="11"/>
@@ -1373,7 +1370,7 @@
       <c r="U3" s="11"/>
       <c r="V3">
         <f t="shared" si="9"/>
-        <v>19.25</v>
+        <v>24.25</v>
       </c>
       <c r="W3">
         <f t="shared" si="10"/>
@@ -1422,32 +1419,32 @@
         <v>9</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M4">
         <f t="shared" si="4"/>
-        <v>-0.5</v>
+        <v>3.25</v>
       </c>
       <c r="N4">
         <f t="shared" si="5"/>
-        <v>-3.3333333333333335</v>
+        <v>21.666666666666668</v>
       </c>
       <c r="O4">
         <f t="shared" si="6"/>
-        <v>10.25</v>
+        <v>14</v>
       </c>
       <c r="P4">
         <f t="shared" si="7"/>
-        <v>14.642857142857144</v>
+        <v>20</v>
       </c>
       <c r="Q4">
         <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="R4" s="19">
+        <v>6</v>
+      </c>
+      <c r="R4" s="10">
         <v>12</v>
       </c>
       <c r="S4" s="11"/>
@@ -1455,11 +1452,11 @@
       <c r="U4" s="11"/>
       <c r="V4">
         <f t="shared" si="9"/>
-        <v>22.25</v>
+        <v>26</v>
       </c>
       <c r="W4">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y4">
         <f>SUM(Y1:Y3)</f>
@@ -1502,32 +1499,32 @@
         <v>15</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M5">
         <f t="shared" si="4"/>
-        <v>0.75</v>
+        <v>3.25</v>
       </c>
       <c r="N5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>21.666666666666668</v>
       </c>
       <c r="O5">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>11.5</v>
       </c>
       <c r="P5">
         <f t="shared" si="7"/>
-        <v>12.857142857142856</v>
+        <v>16.428571428571427</v>
       </c>
       <c r="Q5">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="R5" s="19">
+      <c r="R5" s="10">
         <v>14.5</v>
       </c>
       <c r="S5" s="11"/>
@@ -1535,11 +1532,11 @@
       <c r="U5" s="11"/>
       <c r="V5">
         <f t="shared" si="9"/>
-        <v>23.5</v>
+        <v>26</v>
       </c>
       <c r="W5">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1601,9 +1598,9 @@
       </c>
       <c r="Q6">
         <f t="shared" si="8"/>
-        <v>7</v>
-      </c>
-      <c r="R6" s="19"/>
+        <v>11</v>
+      </c>
+      <c r="R6" s="10"/>
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
@@ -1613,7 +1610,7 @@
       </c>
       <c r="W6">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Y6" t="s">
         <v>31</v>
@@ -1665,7 +1662,7 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R7" s="19"/>
+      <c r="R7" s="10"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
       <c r="U7" s="11"/>
@@ -1714,32 +1711,32 @@
         <v>2</v>
       </c>
       <c r="K8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M8">
         <f t="shared" si="4"/>
-        <v>0.75</v>
+        <v>3.25</v>
       </c>
       <c r="N8">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>21.666666666666668</v>
       </c>
       <c r="O8">
         <f t="shared" si="6"/>
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="P8">
         <f t="shared" si="7"/>
-        <v>10.714285714285714</v>
+        <v>14.285714285714285</v>
       </c>
       <c r="Q8">
         <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="R8" s="19">
+        <v>9</v>
+      </c>
+      <c r="R8" s="10">
         <v>11.5</v>
       </c>
       <c r="S8" s="13"/>
@@ -1747,7 +1744,7 @@
       <c r="U8" s="13"/>
       <c r="V8">
         <f t="shared" si="9"/>
-        <v>19</v>
+        <v>21.5</v>
       </c>
       <c r="W8">
         <f t="shared" si="10"/>
@@ -1790,32 +1787,32 @@
         <v>6</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <f t="shared" si="4"/>
-        <v>-1.25</v>
+        <v>3.75</v>
       </c>
       <c r="N9">
         <f t="shared" si="5"/>
-        <v>-8.3333333333333321</v>
+        <v>25</v>
       </c>
       <c r="O9">
         <f t="shared" si="6"/>
-        <v>4.75</v>
+        <v>9.75</v>
       </c>
       <c r="P9">
         <f t="shared" si="7"/>
-        <v>6.7857142857142856</v>
+        <v>13.928571428571429</v>
       </c>
       <c r="Q9">
         <f t="shared" si="8"/>
-        <v>11</v>
-      </c>
-      <c r="R9" s="19">
+        <v>10</v>
+      </c>
+      <c r="R9" s="10">
         <v>15.5</v>
       </c>
       <c r="S9" s="11"/>
@@ -1823,11 +1820,11 @@
       <c r="U9" s="11"/>
       <c r="V9">
         <f t="shared" si="9"/>
-        <v>20.25</v>
+        <v>25.25</v>
       </c>
       <c r="W9">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1866,32 +1863,32 @@
         <v>21</v>
       </c>
       <c r="K10">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M10">
         <f t="shared" si="4"/>
-        <v>3.25</v>
+        <v>8.25</v>
       </c>
       <c r="N10">
         <f t="shared" si="5"/>
-        <v>21.666666666666668</v>
+        <v>55.000000000000007</v>
       </c>
       <c r="O10">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="P10">
         <f t="shared" si="7"/>
-        <v>20</v>
+        <v>27.142857142857142</v>
       </c>
       <c r="Q10">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="R10" s="19">
+      <c r="R10" s="10">
         <v>9.5</v>
       </c>
       <c r="S10" s="13"/>
@@ -1899,7 +1896,7 @@
       <c r="U10" s="13"/>
       <c r="V10">
         <f t="shared" si="9"/>
-        <v>23.5</v>
+        <v>28.5</v>
       </c>
       <c r="W10">
         <f t="shared" si="10"/>
@@ -1949,7 +1946,7 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R11" s="19"/>
+      <c r="R11" s="10"/>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
       <c r="U11" s="11"/>
@@ -2005,7 +2002,7 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R12" s="19"/>
+      <c r="R12" s="10"/>
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
@@ -2075,7 +2072,7 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R13" s="19">
+      <c r="R13" s="10">
         <v>9</v>
       </c>
       <c r="S13" s="13"/>
@@ -2087,7 +2084,7 @@
       </c>
       <c r="W13">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -2133,7 +2130,7 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R14" s="19"/>
+      <c r="R14" s="10"/>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
@@ -2189,7 +2186,7 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R15" s="19"/>
+      <c r="R15" s="10"/>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
       <c r="U15" s="11"/>
@@ -2245,7 +2242,7 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R16" s="19"/>
+      <c r="R16" s="10"/>
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
       <c r="U16" s="11"/>
@@ -2301,7 +2298,7 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R17" s="19"/>
+      <c r="R17" s="10"/>
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
       <c r="U17" s="11"/>
@@ -2357,7 +2354,7 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R18" s="19"/>
+      <c r="R18" s="10"/>
       <c r="S18" s="13"/>
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
@@ -2406,32 +2403,32 @@
         <v>-13</v>
       </c>
       <c r="K19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L19">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M19">
         <f t="shared" si="4"/>
-        <v>-0.75</v>
+        <v>3</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
-        <v>-5</v>
+        <v>20</v>
       </c>
       <c r="O19">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-0.25</v>
       </c>
       <c r="P19">
         <f t="shared" si="7"/>
-        <v>-5.7142857142857144</v>
+        <v>-0.35714285714285715</v>
       </c>
       <c r="Q19">
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="R19" s="19">
+      <c r="R19" s="10">
         <v>12</v>
       </c>
       <c r="S19" s="11"/>
@@ -2439,11 +2436,11 @@
       <c r="U19" s="11"/>
       <c r="V19">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>11.75</v>
       </c>
       <c r="W19">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -2489,7 +2486,7 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R20" s="19"/>
+      <c r="R20" s="10"/>
       <c r="S20" s="11"/>
       <c r="T20" s="11"/>
       <c r="U20" s="11"/>
@@ -2538,32 +2535,32 @@
         <v>8</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L21">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M21">
         <f t="shared" si="14"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
-        <v>-6.666666666666667</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="O21">
         <f t="shared" si="6"/>
-        <v>10.25</v>
+        <v>15.25</v>
       </c>
       <c r="P21">
         <f t="shared" si="7"/>
-        <v>14.642857142857144</v>
+        <v>21.785714285714285</v>
       </c>
       <c r="Q21">
         <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="R21" s="19">
+        <v>4</v>
+      </c>
+      <c r="R21" s="10">
         <v>18.5</v>
       </c>
       <c r="S21" s="11"/>
@@ -2571,7 +2568,7 @@
       <c r="U21" s="11"/>
       <c r="V21">
         <f t="shared" si="11"/>
-        <v>28.75</v>
+        <v>33.75</v>
       </c>
       <c r="W21">
         <f t="shared" si="10"/>
@@ -2614,32 +2611,32 @@
         <v>16</v>
       </c>
       <c r="K22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L22">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M22">
         <f t="shared" si="14"/>
-        <v>1.25</v>
+        <v>3.75</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
-        <v>8.3333333333333321</v>
+        <v>25</v>
       </c>
       <c r="O22">
         <f t="shared" si="6"/>
-        <v>12.25</v>
+        <v>14.75</v>
       </c>
       <c r="P22">
         <f t="shared" si="7"/>
-        <v>17.5</v>
+        <v>21.071428571428573</v>
       </c>
       <c r="Q22">
         <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="R22" s="19">
+        <v>5</v>
+      </c>
+      <c r="R22" s="10">
         <v>10</v>
       </c>
       <c r="S22" s="11"/>
@@ -2647,11 +2644,11 @@
       <c r="U22" s="11"/>
       <c r="V22">
         <f t="shared" si="11"/>
-        <v>22.25</v>
+        <v>24.75</v>
       </c>
       <c r="W22">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="43.8" customHeight="1" thickBot="1">
@@ -2690,32 +2687,32 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M23">
         <f t="shared" si="14"/>
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
-        <v>1.6666666666666667</v>
+        <v>10</v>
       </c>
       <c r="O23">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4.25</v>
       </c>
       <c r="P23">
         <f t="shared" si="7"/>
-        <v>4.2857142857142856</v>
+        <v>6.0714285714285712</v>
       </c>
       <c r="Q23">
         <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="R23" s="19">
+        <v>13</v>
+      </c>
+      <c r="R23" s="10">
         <v>13</v>
       </c>
       <c r="S23" s="11"/>
@@ -2723,7 +2720,7 @@
       <c r="U23" s="11"/>
       <c r="V23">
         <f t="shared" si="11"/>
-        <v>16</v>
+        <v>17.25</v>
       </c>
       <c r="W23">
         <f t="shared" si="10"/>
@@ -2766,32 +2763,32 @@
         <v>40</v>
       </c>
       <c r="K24">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L24">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M24">
         <f t="shared" si="14"/>
-        <v>1.5</v>
+        <v>6.5</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>43.333333333333336</v>
       </c>
       <c r="O24">
         <f t="shared" si="6"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="P24">
         <f t="shared" si="7"/>
-        <v>35.714285714285715</v>
+        <v>42.857142857142854</v>
       </c>
       <c r="Q24">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="R24" s="19">
+      <c r="R24" s="10">
         <v>20</v>
       </c>
       <c r="S24" s="11"/>
@@ -2799,7 +2796,7 @@
       <c r="U24" s="11"/>
       <c r="V24">
         <f t="shared" si="11"/>
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="W24">
         <f t="shared" si="10"/>
@@ -2842,32 +2839,32 @@
         <v>20</v>
       </c>
       <c r="K25">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M25">
         <f t="shared" si="14"/>
-        <v>1.75</v>
+        <v>6.75</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
-        <v>11.666666666666666</v>
+        <v>45</v>
       </c>
       <c r="O25">
         <f t="shared" si="6"/>
-        <v>20.25</v>
+        <v>25.25</v>
       </c>
       <c r="P25">
         <f t="shared" si="7"/>
-        <v>28.928571428571431</v>
+        <v>36.071428571428569</v>
       </c>
       <c r="Q25">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="R25" s="19">
+      <c r="R25" s="10">
         <v>22.5</v>
       </c>
       <c r="S25" s="11"/>
@@ -2875,7 +2872,7 @@
       <c r="U25" s="11"/>
       <c r="V25">
         <f t="shared" si="11"/>
-        <v>42.75</v>
+        <v>47.75</v>
       </c>
       <c r="W25">
         <f t="shared" si="10"/>

</xml_diff>